<commit_message>
added graphs for mandelbrot & tricorn
</commit_message>
<xml_diff>
--- a/pthreads/fractal_performance_measurement.xlsx
+++ b/pthreads/fractal_performance_measurement.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fractal_proj\pthreads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF324EE-78BB-4C55-B76D-14890582A7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1CBC9-FCE6-464B-9469-3856819D92FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4C170DF-AD9F-4F5F-BF83-86F9507F060A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B4C170DF-AD9F-4F5F-BF83-86F9507F060A}"/>
   </bookViews>
   <sheets>
     <sheet name="Julia results" sheetId="1" r:id="rId1"/>
+    <sheet name="Mandelbrot results" sheetId="2" r:id="rId2"/>
+    <sheet name="Tricorn results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>Number of threads</t>
   </si>
@@ -355,6 +357,1020 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-18B7-4A52-9EA4-34D1665C9ACA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="846926223"/>
+        <c:axId val="846925743"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="846926223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="55"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of threads</a:t>
+                </a:r>
+                <a:endParaRPr lang="ro-RO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ro-RO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846925743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="846925743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ro-RO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ro-RO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846926223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ro-RO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Execution Time for Mandelbrot fractal</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ro-RO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>execution time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Mandelbrot results'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Mandelbrot results'!$B$3:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1504.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>865.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>809.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>828.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>580.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>527.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>442.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>428.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>398.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>399.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>368.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>362.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CB2A-48D5-A649-2CCD25883576}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="846926223"/>
+        <c:axId val="846925743"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="846926223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="55"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of threads</a:t>
+                </a:r>
+                <a:endParaRPr lang="ro-RO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ro-RO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846925743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="846925743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ro-RO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ro-RO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="846926223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ro-RO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Execution Time for Tricorn fractal</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ro-RO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>execution time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tricorn results'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tricorn results'!$B$3:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>597.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>407.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>368.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>432.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>329.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>325.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>309.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>278.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>269.10000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADC9-45A1-9523-56C1F183846E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -702,7 +1718,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1230,6 +3332,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{737132C3-9405-45ED-A875-F677E7019920}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C851D995-AF2A-4A09-A04B-1E87F4079244}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1565,14 +3753,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C541E42E-6909-4F78-B90E-F33F7F403FC6}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
@@ -2092,4 +4280,1088 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087AD78D-1A6D-4904-9DD2-20A2C3191B5C}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <f>AVERAGE(C3:L3)</f>
+        <v>1504.1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1503</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1525</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1474</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1516</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1518</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1507</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1529</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1487</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1482</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B14" si="0">AVERAGE(C4:L4)</f>
+        <v>865.2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>876</v>
+      </c>
+      <c r="D4" s="3">
+        <v>869</v>
+      </c>
+      <c r="E4" s="3">
+        <v>855</v>
+      </c>
+      <c r="F4" s="3">
+        <v>858</v>
+      </c>
+      <c r="G4" s="3">
+        <v>864</v>
+      </c>
+      <c r="H4" s="3">
+        <v>866</v>
+      </c>
+      <c r="I4" s="3">
+        <v>883</v>
+      </c>
+      <c r="J4" s="3">
+        <v>860</v>
+      </c>
+      <c r="K4" s="3">
+        <v>859</v>
+      </c>
+      <c r="L4" s="3">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>809.8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>791</v>
+      </c>
+      <c r="D5" s="3">
+        <v>811</v>
+      </c>
+      <c r="E5" s="3">
+        <v>818</v>
+      </c>
+      <c r="F5" s="3">
+        <v>827</v>
+      </c>
+      <c r="G5" s="3">
+        <v>798</v>
+      </c>
+      <c r="H5" s="3">
+        <v>818</v>
+      </c>
+      <c r="I5" s="3">
+        <v>808</v>
+      </c>
+      <c r="J5" s="3">
+        <v>809</v>
+      </c>
+      <c r="K5" s="3">
+        <v>806</v>
+      </c>
+      <c r="L5" s="3">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>828.9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>829</v>
+      </c>
+      <c r="D6" s="3">
+        <v>814</v>
+      </c>
+      <c r="E6" s="3">
+        <v>830</v>
+      </c>
+      <c r="F6" s="3">
+        <v>825</v>
+      </c>
+      <c r="G6" s="3">
+        <v>836</v>
+      </c>
+      <c r="H6" s="3">
+        <v>833</v>
+      </c>
+      <c r="I6" s="3">
+        <v>827</v>
+      </c>
+      <c r="J6" s="3">
+        <v>832</v>
+      </c>
+      <c r="K6" s="3">
+        <v>834</v>
+      </c>
+      <c r="L6" s="3">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>580.6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>586</v>
+      </c>
+      <c r="D7" s="3">
+        <v>576</v>
+      </c>
+      <c r="E7" s="3">
+        <v>580</v>
+      </c>
+      <c r="F7" s="3">
+        <v>587</v>
+      </c>
+      <c r="G7" s="3">
+        <v>568</v>
+      </c>
+      <c r="H7" s="3">
+        <v>581</v>
+      </c>
+      <c r="I7" s="3">
+        <v>586</v>
+      </c>
+      <c r="J7" s="3">
+        <v>584</v>
+      </c>
+      <c r="K7" s="3">
+        <v>587</v>
+      </c>
+      <c r="L7" s="3">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>527.5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>533</v>
+      </c>
+      <c r="D8" s="3">
+        <v>528</v>
+      </c>
+      <c r="E8" s="3">
+        <v>531</v>
+      </c>
+      <c r="F8" s="3">
+        <v>519</v>
+      </c>
+      <c r="G8" s="3">
+        <v>521</v>
+      </c>
+      <c r="H8" s="3">
+        <v>530</v>
+      </c>
+      <c r="I8" s="3">
+        <v>528</v>
+      </c>
+      <c r="J8" s="3">
+        <v>529</v>
+      </c>
+      <c r="K8" s="3">
+        <v>532</v>
+      </c>
+      <c r="L8" s="3">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>442.1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>428</v>
+      </c>
+      <c r="D9" s="3">
+        <v>446</v>
+      </c>
+      <c r="E9" s="3">
+        <v>452</v>
+      </c>
+      <c r="F9" s="3">
+        <v>451</v>
+      </c>
+      <c r="G9" s="3">
+        <v>444</v>
+      </c>
+      <c r="H9" s="3">
+        <v>434</v>
+      </c>
+      <c r="I9" s="3">
+        <v>447</v>
+      </c>
+      <c r="J9" s="3">
+        <v>448</v>
+      </c>
+      <c r="K9" s="3">
+        <v>436</v>
+      </c>
+      <c r="L9" s="3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>428.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>425</v>
+      </c>
+      <c r="D10" s="3">
+        <v>429</v>
+      </c>
+      <c r="E10" s="3">
+        <v>432</v>
+      </c>
+      <c r="F10" s="3">
+        <v>428</v>
+      </c>
+      <c r="G10" s="3">
+        <v>432</v>
+      </c>
+      <c r="H10" s="3">
+        <v>417</v>
+      </c>
+      <c r="I10" s="3">
+        <v>433</v>
+      </c>
+      <c r="J10" s="3">
+        <v>424</v>
+      </c>
+      <c r="K10" s="3">
+        <v>435</v>
+      </c>
+      <c r="L10" s="3">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>398.4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>377</v>
+      </c>
+      <c r="D11" s="3">
+        <v>399</v>
+      </c>
+      <c r="E11" s="3">
+        <v>411</v>
+      </c>
+      <c r="F11" s="3">
+        <v>416</v>
+      </c>
+      <c r="G11" s="3">
+        <v>413</v>
+      </c>
+      <c r="H11" s="3">
+        <v>386</v>
+      </c>
+      <c r="I11" s="3">
+        <v>402</v>
+      </c>
+      <c r="J11" s="3">
+        <v>406</v>
+      </c>
+      <c r="K11" s="3">
+        <v>370</v>
+      </c>
+      <c r="L11" s="3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>399.8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>401</v>
+      </c>
+      <c r="D12" s="3">
+        <v>409</v>
+      </c>
+      <c r="E12" s="3">
+        <v>367</v>
+      </c>
+      <c r="F12" s="3">
+        <v>403</v>
+      </c>
+      <c r="G12" s="3">
+        <v>405</v>
+      </c>
+      <c r="H12" s="3">
+        <v>397</v>
+      </c>
+      <c r="I12" s="3">
+        <v>407</v>
+      </c>
+      <c r="J12" s="3">
+        <v>411</v>
+      </c>
+      <c r="K12" s="3">
+        <v>400</v>
+      </c>
+      <c r="L12" s="3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>368.8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>389</v>
+      </c>
+      <c r="D13" s="3">
+        <v>394</v>
+      </c>
+      <c r="E13" s="3">
+        <v>373</v>
+      </c>
+      <c r="F13" s="3">
+        <v>349</v>
+      </c>
+      <c r="G13" s="3">
+        <v>380</v>
+      </c>
+      <c r="H13" s="3">
+        <v>344</v>
+      </c>
+      <c r="I13" s="3">
+        <v>342</v>
+      </c>
+      <c r="J13" s="3">
+        <v>379</v>
+      </c>
+      <c r="K13" s="3">
+        <v>382</v>
+      </c>
+      <c r="L13" s="3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>362.2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>379</v>
+      </c>
+      <c r="D14" s="3">
+        <v>354</v>
+      </c>
+      <c r="E14" s="3">
+        <v>341</v>
+      </c>
+      <c r="F14" s="3">
+        <v>382</v>
+      </c>
+      <c r="G14" s="3">
+        <v>376</v>
+      </c>
+      <c r="H14" s="3">
+        <v>364</v>
+      </c>
+      <c r="I14" s="3">
+        <v>342</v>
+      </c>
+      <c r="J14" s="3">
+        <v>345</v>
+      </c>
+      <c r="K14" s="3">
+        <v>366</v>
+      </c>
+      <c r="L14" s="3">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A043122-CAB2-477F-87EF-F1BABC3D58B5}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <f>AVERAGE(C3:L3)</f>
+        <v>597.1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>592</v>
+      </c>
+      <c r="D3" s="3">
+        <v>596</v>
+      </c>
+      <c r="E3" s="3">
+        <v>594</v>
+      </c>
+      <c r="F3" s="3">
+        <v>603</v>
+      </c>
+      <c r="G3" s="3">
+        <v>596</v>
+      </c>
+      <c r="H3" s="3">
+        <v>604</v>
+      </c>
+      <c r="I3" s="3">
+        <v>599</v>
+      </c>
+      <c r="J3" s="3">
+        <v>599</v>
+      </c>
+      <c r="K3" s="3">
+        <v>592</v>
+      </c>
+      <c r="L3" s="3">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B14" si="0">AVERAGE(C4:L4)</f>
+        <v>407.6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>395</v>
+      </c>
+      <c r="D4" s="3">
+        <v>407</v>
+      </c>
+      <c r="E4" s="3">
+        <v>410</v>
+      </c>
+      <c r="F4" s="3">
+        <v>410</v>
+      </c>
+      <c r="G4" s="3">
+        <v>413</v>
+      </c>
+      <c r="H4" s="3">
+        <v>415</v>
+      </c>
+      <c r="I4" s="3">
+        <v>402</v>
+      </c>
+      <c r="J4" s="3">
+        <v>406</v>
+      </c>
+      <c r="K4" s="3">
+        <v>410</v>
+      </c>
+      <c r="L4" s="3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>368.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>370</v>
+      </c>
+      <c r="D5" s="3">
+        <v>366</v>
+      </c>
+      <c r="E5" s="3">
+        <v>379</v>
+      </c>
+      <c r="F5" s="3">
+        <v>376</v>
+      </c>
+      <c r="G5" s="3">
+        <v>358</v>
+      </c>
+      <c r="H5" s="3">
+        <v>373</v>
+      </c>
+      <c r="I5" s="3">
+        <v>376</v>
+      </c>
+      <c r="J5" s="3">
+        <v>370</v>
+      </c>
+      <c r="K5" s="3">
+        <v>348</v>
+      </c>
+      <c r="L5" s="3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>432.4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>436</v>
+      </c>
+      <c r="D6" s="3">
+        <v>442</v>
+      </c>
+      <c r="E6" s="3">
+        <v>437</v>
+      </c>
+      <c r="F6" s="3">
+        <v>412</v>
+      </c>
+      <c r="G6" s="3">
+        <v>434</v>
+      </c>
+      <c r="H6" s="3">
+        <v>435</v>
+      </c>
+      <c r="I6" s="3">
+        <v>442</v>
+      </c>
+      <c r="J6" s="3">
+        <v>424</v>
+      </c>
+      <c r="K6" s="3">
+        <v>430</v>
+      </c>
+      <c r="L6" s="3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>329.4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>332</v>
+      </c>
+      <c r="D7" s="3">
+        <v>316</v>
+      </c>
+      <c r="E7" s="3">
+        <v>334</v>
+      </c>
+      <c r="F7" s="3">
+        <v>330</v>
+      </c>
+      <c r="G7" s="3">
+        <v>332</v>
+      </c>
+      <c r="H7" s="3">
+        <v>334</v>
+      </c>
+      <c r="I7" s="3">
+        <v>315</v>
+      </c>
+      <c r="J7" s="3">
+        <v>333</v>
+      </c>
+      <c r="K7" s="3">
+        <v>334</v>
+      </c>
+      <c r="L7" s="3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>325.2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>328</v>
+      </c>
+      <c r="D8" s="3">
+        <v>330</v>
+      </c>
+      <c r="E8" s="3">
+        <v>317</v>
+      </c>
+      <c r="F8" s="3">
+        <v>321</v>
+      </c>
+      <c r="G8" s="3">
+        <v>325</v>
+      </c>
+      <c r="H8" s="3">
+        <v>319</v>
+      </c>
+      <c r="I8" s="3">
+        <v>330</v>
+      </c>
+      <c r="J8" s="3">
+        <v>324</v>
+      </c>
+      <c r="K8" s="3">
+        <v>331</v>
+      </c>
+      <c r="L8" s="3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>309.8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>311</v>
+      </c>
+      <c r="D9" s="3">
+        <v>311</v>
+      </c>
+      <c r="E9" s="3">
+        <v>296</v>
+      </c>
+      <c r="F9" s="3">
+        <v>311</v>
+      </c>
+      <c r="G9" s="3">
+        <v>316</v>
+      </c>
+      <c r="H9" s="3">
+        <v>313</v>
+      </c>
+      <c r="I9" s="3">
+        <v>305</v>
+      </c>
+      <c r="J9" s="3">
+        <v>313</v>
+      </c>
+      <c r="K9" s="3">
+        <v>310</v>
+      </c>
+      <c r="L9" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>308.10000000000002</v>
+      </c>
+      <c r="C10" s="3">
+        <v>309</v>
+      </c>
+      <c r="D10" s="3">
+        <v>308</v>
+      </c>
+      <c r="E10" s="3">
+        <v>311</v>
+      </c>
+      <c r="F10" s="3">
+        <v>312</v>
+      </c>
+      <c r="G10" s="3">
+        <v>308</v>
+      </c>
+      <c r="H10" s="3">
+        <v>312</v>
+      </c>
+      <c r="I10" s="3">
+        <v>308</v>
+      </c>
+      <c r="J10" s="3">
+        <v>305</v>
+      </c>
+      <c r="K10" s="3">
+        <v>300</v>
+      </c>
+      <c r="L10" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>300.89999999999998</v>
+      </c>
+      <c r="C11" s="3">
+        <v>286</v>
+      </c>
+      <c r="D11" s="3">
+        <v>279</v>
+      </c>
+      <c r="E11" s="3">
+        <v>316</v>
+      </c>
+      <c r="F11" s="3">
+        <v>318</v>
+      </c>
+      <c r="G11" s="3">
+        <v>285</v>
+      </c>
+      <c r="H11" s="3">
+        <v>315</v>
+      </c>
+      <c r="I11" s="3">
+        <v>306</v>
+      </c>
+      <c r="J11" s="3">
+        <v>279</v>
+      </c>
+      <c r="K11" s="3">
+        <v>315</v>
+      </c>
+      <c r="L11" s="3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>286</v>
+      </c>
+      <c r="C12" s="3">
+        <v>291</v>
+      </c>
+      <c r="D12" s="3">
+        <v>278</v>
+      </c>
+      <c r="E12" s="3">
+        <v>294</v>
+      </c>
+      <c r="F12" s="3">
+        <v>296</v>
+      </c>
+      <c r="G12" s="3">
+        <v>262</v>
+      </c>
+      <c r="H12" s="3">
+        <v>287</v>
+      </c>
+      <c r="I12" s="3">
+        <v>291</v>
+      </c>
+      <c r="J12" s="3">
+        <v>285</v>
+      </c>
+      <c r="K12" s="3">
+        <v>291</v>
+      </c>
+      <c r="L12" s="3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>278.10000000000002</v>
+      </c>
+      <c r="C13" s="3">
+        <v>277</v>
+      </c>
+      <c r="D13" s="3">
+        <v>287</v>
+      </c>
+      <c r="E13" s="3">
+        <v>291</v>
+      </c>
+      <c r="F13" s="3">
+        <v>285</v>
+      </c>
+      <c r="G13" s="3">
+        <v>263</v>
+      </c>
+      <c r="H13" s="3">
+        <v>288</v>
+      </c>
+      <c r="I13" s="3">
+        <v>263</v>
+      </c>
+      <c r="J13" s="3">
+        <v>288</v>
+      </c>
+      <c r="K13" s="3">
+        <v>263</v>
+      </c>
+      <c r="L13" s="3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>269.10000000000002</v>
+      </c>
+      <c r="C14" s="3">
+        <v>276</v>
+      </c>
+      <c r="D14" s="3">
+        <v>285</v>
+      </c>
+      <c r="E14" s="3">
+        <v>259</v>
+      </c>
+      <c r="F14" s="3">
+        <v>267</v>
+      </c>
+      <c r="G14" s="3">
+        <v>267</v>
+      </c>
+      <c r="H14" s="3">
+        <v>271</v>
+      </c>
+      <c r="I14" s="3">
+        <v>273</v>
+      </c>
+      <c r="J14" s="3">
+        <v>281</v>
+      </c>
+      <c r="K14" s="3">
+        <v>240</v>
+      </c>
+      <c r="L14" s="3">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>